<commit_message>
fix data siswa&& update db
</commit_message>
<xml_diff>
--- a/public/file_siswa/template-data-siswa.xlsx
+++ b/public/file_siswa/template-data-siswa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lab Unama\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D5ECCE-32DD-484C-8255-6E33C7BAC7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC304536-87DE-49F4-BEA1-FF6F8E3B8453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="52">
   <si>
     <t>Aldi Taher</t>
   </si>
@@ -162,6 +162,33 @@
   </si>
   <si>
     <t>2022-05-31</t>
+  </si>
+  <si>
+    <t>Alamat</t>
+  </si>
+  <si>
+    <t>Program Studi</t>
+  </si>
+  <si>
+    <t>Durasi</t>
+  </si>
+  <si>
+    <t>Jambi</t>
+  </si>
+  <si>
+    <t>Fashion Design</t>
+  </si>
+  <si>
+    <t>Menjahit</t>
+  </si>
+  <si>
+    <t>3 bulan</t>
+  </si>
+  <si>
+    <t>6 bulan</t>
+  </si>
+  <si>
+    <t>12 bulan</t>
   </si>
 </sst>
 </file>
@@ -519,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" activeCellId="3" sqref="F14 F15 F16 F17"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,9 +560,12 @@
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -554,8 +584,17 @@
       <c r="F1" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -574,8 +613,17 @@
       <c r="F2" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -594,8 +642,17 @@
       <c r="F3" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -614,8 +671,17 @@
       <c r="F4" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -634,8 +700,17 @@
       <c r="F5" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -654,8 +729,17 @@
       <c r="F6" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -674,8 +758,17 @@
       <c r="F7" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -694,8 +787,17 @@
       <c r="F8" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -714,8 +816,17 @@
       <c r="F9" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -734,8 +845,17 @@
       <c r="F10" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -754,8 +874,17 @@
       <c r="F11" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -774,8 +903,17 @@
       <c r="F12" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -794,8 +932,17 @@
       <c r="F13" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -814,8 +961,17 @@
       <c r="F14" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -834,8 +990,17 @@
       <c r="F15" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -854,8 +1019,17 @@
       <c r="F16" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -873,6 +1047,15 @@
       </c>
       <c r="F17" s="5" t="s">
         <v>42</v>
+      </c>
+      <c r="G17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>